<commit_message>
Complete dashboard optimization and bug fixes - all features working
Co-authored-by: robertopotenza <138742974+robertopotenza@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A215"/>
+  <dimension ref="A1:A216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1938,6 +1938,13 @@
         </is>
       </c>
     </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>TESLAX</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Complete extractor debug validation with comprehensive guide and improved gitignore
Co-authored-by: robertopotenza <138742974+robertopotenza@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-24T14:49:03.996309</t>
+          <t>2025-09-24T14:51:49.538477</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -629,77 +629,27 @@
           <t>AAPL</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/apple-computer-inc-technical</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-09-24T14:49:04.896341</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>234</v>
-      </c>
-      <c r="G3" t="n">
-        <v>225</v>
-      </c>
-      <c r="H3" t="n">
-        <v>215</v>
-      </c>
-      <c r="I3" t="n">
-        <v>259</v>
-      </c>
-      <c r="J3" t="n">
-        <v>269</v>
-      </c>
-      <c r="K3" t="n">
-        <v>239</v>
-      </c>
-      <c r="L3" t="n">
-        <v>238</v>
-      </c>
-      <c r="M3" t="n">
-        <v>52</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-8</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-5.5</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>264</v>
-      </c>
-      <c r="R3" t="n">
-        <v>242</v>
-      </c>
-      <c r="S3" t="n">
-        <v>220</v>
-      </c>
-      <c r="T3" t="n">
-        <v>4140142</v>
-      </c>
-      <c r="U3" t="n">
-        <v>62</v>
-      </c>
-      <c r="V3" t="n">
-        <v>3</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">

</xml_diff>

<commit_message>
Add Technical Indicators dashboard section with complete data display
Co-authored-by: robertopotenza <138742974+robertopotenza@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-24T14:49:03.996309</t>
+          <t>2025-09-24T15:10:35.335491</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-09-24T14:49:04.896341</t>
+          <t>2025-09-24T15:10:37.042674</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -707,27 +707,77 @@
           <t>ABBV</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/abbvie-inc-technical</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:38.971697</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>354</v>
+      </c>
+      <c r="G4" t="n">
+        <v>345</v>
+      </c>
+      <c r="H4" t="n">
+        <v>325</v>
+      </c>
+      <c r="I4" t="n">
+        <v>379</v>
+      </c>
+      <c r="J4" t="n">
+        <v>399</v>
+      </c>
+      <c r="K4" t="n">
+        <v>359</v>
+      </c>
+      <c r="L4" t="n">
+        <v>362</v>
+      </c>
+      <c r="M4" t="n">
+        <v>32</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-8</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-2</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>384</v>
+      </c>
+      <c r="R4" t="n">
+        <v>362</v>
+      </c>
+      <c r="S4" t="n">
+        <v>340</v>
+      </c>
+      <c r="T4" t="n">
+        <v>2709762</v>
+      </c>
+      <c r="U4" t="n">
+        <v>32</v>
+      </c>
+      <c r="V4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -735,27 +785,77 @@
           <t>ADBE</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/adobe-inc-technical</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:40.686815</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>176</v>
+      </c>
+      <c r="G5" t="n">
+        <v>165</v>
+      </c>
+      <c r="H5" t="n">
+        <v>155</v>
+      </c>
+      <c r="I5" t="n">
+        <v>201</v>
+      </c>
+      <c r="J5" t="n">
+        <v>211</v>
+      </c>
+      <c r="K5" t="n">
+        <v>181</v>
+      </c>
+      <c r="L5" t="n">
+        <v>180</v>
+      </c>
+      <c r="M5" t="n">
+        <v>53</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-7</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>206</v>
+      </c>
+      <c r="R5" t="n">
+        <v>183</v>
+      </c>
+      <c r="S5" t="n">
+        <v>160</v>
+      </c>
+      <c r="T5" t="n">
+        <v>8699583</v>
+      </c>
+      <c r="U5" t="n">
+        <v>53</v>
+      </c>
+      <c r="V5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -763,27 +863,77 @@
           <t>ADI</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/analog-devices-technical</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:42.673470</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>274</v>
+      </c>
+      <c r="G6" t="n">
+        <v>255</v>
+      </c>
+      <c r="H6" t="n">
+        <v>240</v>
+      </c>
+      <c r="I6" t="n">
+        <v>289</v>
+      </c>
+      <c r="J6" t="n">
+        <v>304</v>
+      </c>
+      <c r="K6" t="n">
+        <v>269</v>
+      </c>
+      <c r="L6" t="n">
+        <v>270</v>
+      </c>
+      <c r="M6" t="n">
+        <v>62</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-4</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>294</v>
+      </c>
+      <c r="R6" t="n">
+        <v>272</v>
+      </c>
+      <c r="S6" t="n">
+        <v>250</v>
+      </c>
+      <c r="T6" t="n">
+        <v>10933672</v>
+      </c>
+      <c r="U6" t="n">
+        <v>42</v>
+      </c>
+      <c r="V6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -791,27 +941,77 @@
           <t>ADSK</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/autodesk-inc-technical</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:43.838381</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>112</v>
+      </c>
+      <c r="G7" t="n">
+        <v>95</v>
+      </c>
+      <c r="H7" t="n">
+        <v>80</v>
+      </c>
+      <c r="I7" t="n">
+        <v>127</v>
+      </c>
+      <c r="J7" t="n">
+        <v>142</v>
+      </c>
+      <c r="K7" t="n">
+        <v>107</v>
+      </c>
+      <c r="L7" t="n">
+        <v>108</v>
+      </c>
+      <c r="M7" t="n">
+        <v>41</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>132</v>
+      </c>
+      <c r="R7" t="n">
+        <v>111</v>
+      </c>
+      <c r="S7" t="n">
+        <v>90</v>
+      </c>
+      <c r="T7" t="n">
+        <v>6281011</v>
+      </c>
+      <c r="U7" t="n">
+        <v>31</v>
+      </c>
+      <c r="V7" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -819,27 +1019,77 @@
           <t>ADYEY</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/adyen-nv-otc-technical</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:45.441807</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>226</v>
+      </c>
+      <c r="G8" t="n">
+        <v>195</v>
+      </c>
+      <c r="H8" t="n">
+        <v>190</v>
+      </c>
+      <c r="I8" t="n">
+        <v>241</v>
+      </c>
+      <c r="J8" t="n">
+        <v>246</v>
+      </c>
+      <c r="K8" t="n">
+        <v>221</v>
+      </c>
+      <c r="L8" t="n">
+        <v>218</v>
+      </c>
+      <c r="M8" t="n">
+        <v>48</v>
+      </c>
+      <c r="N8" t="n">
+        <v>8</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-2</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>246</v>
+      </c>
+      <c r="R8" t="n">
+        <v>218</v>
+      </c>
+      <c r="S8" t="n">
+        <v>190</v>
+      </c>
+      <c r="T8" t="n">
+        <v>5834618</v>
+      </c>
+      <c r="U8" t="n">
+        <v>38</v>
+      </c>
+      <c r="V8" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -847,27 +1097,77 @@
           <t>AEM</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/agnico-eagle-mines-technical</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:47.092396</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>402</v>
+      </c>
+      <c r="G9" t="n">
+        <v>385</v>
+      </c>
+      <c r="H9" t="n">
+        <v>375</v>
+      </c>
+      <c r="I9" t="n">
+        <v>427</v>
+      </c>
+      <c r="J9" t="n">
+        <v>437</v>
+      </c>
+      <c r="K9" t="n">
+        <v>407</v>
+      </c>
+      <c r="L9" t="n">
+        <v>406</v>
+      </c>
+      <c r="M9" t="n">
+        <v>36</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-4</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>432</v>
+      </c>
+      <c r="R9" t="n">
+        <v>406</v>
+      </c>
+      <c r="S9" t="n">
+        <v>380</v>
+      </c>
+      <c r="T9" t="n">
+        <v>8205806</v>
+      </c>
+      <c r="U9" t="n">
+        <v>26</v>
+      </c>
+      <c r="V9" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -875,27 +1175,77 @@
           <t>AJG</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/arthur-j.-gallagher---co-technical</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:48.502007</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>450</v>
+      </c>
+      <c r="G10" t="n">
+        <v>435</v>
+      </c>
+      <c r="H10" t="n">
+        <v>420</v>
+      </c>
+      <c r="I10" t="n">
+        <v>465</v>
+      </c>
+      <c r="J10" t="n">
+        <v>480</v>
+      </c>
+      <c r="K10" t="n">
+        <v>445</v>
+      </c>
+      <c r="L10" t="n">
+        <v>446</v>
+      </c>
+      <c r="M10" t="n">
+        <v>60</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="P10" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>470</v>
+      </c>
+      <c r="R10" t="n">
+        <v>450</v>
+      </c>
+      <c r="S10" t="n">
+        <v>430</v>
+      </c>
+      <c r="T10" t="n">
+        <v>4003350</v>
+      </c>
+      <c r="U10" t="n">
+        <v>20</v>
+      </c>
+      <c r="V10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -903,27 +1253,77 @@
           <t>ALL</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.investing.com/equities/allstate-corp-technical</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-09-24T15:10:50.048240</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>mock</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Mock data used due to network unavailability</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>312</v>
+      </c>
+      <c r="G11" t="n">
+        <v>305</v>
+      </c>
+      <c r="H11" t="n">
+        <v>290</v>
+      </c>
+      <c r="I11" t="n">
+        <v>337</v>
+      </c>
+      <c r="J11" t="n">
+        <v>352</v>
+      </c>
+      <c r="K11" t="n">
+        <v>317</v>
+      </c>
+      <c r="L11" t="n">
+        <v>324</v>
+      </c>
+      <c r="M11" t="n">
+        <v>51</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-9</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>342</v>
+      </c>
+      <c r="R11" t="n">
+        <v>321</v>
+      </c>
+      <c r="S11" t="n">
+        <v>300</v>
+      </c>
+      <c r="T11" t="n">
+        <v>6499221</v>
+      </c>
+      <c r="U11" t="n">
+        <v>41</v>
+      </c>
+      <c r="V11" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">

</xml_diff>

<commit_message>
Initial debugging analysis - identified DNS resolution issue
Co-authored-by: robertopotenza <138742974+robertopotenza@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-24T15:10:35.335491</t>
+          <t>2025-09-24T19:34:13.184636</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -629,77 +629,27 @@
           <t>AAPL</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/apple-computer-inc-technical</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:37.042674</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>234</v>
-      </c>
-      <c r="G3" t="n">
-        <v>225</v>
-      </c>
-      <c r="H3" t="n">
-        <v>215</v>
-      </c>
-      <c r="I3" t="n">
-        <v>259</v>
-      </c>
-      <c r="J3" t="n">
-        <v>269</v>
-      </c>
-      <c r="K3" t="n">
-        <v>239</v>
-      </c>
-      <c r="L3" t="n">
-        <v>238</v>
-      </c>
-      <c r="M3" t="n">
-        <v>52</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-8</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-5.5</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>264</v>
-      </c>
-      <c r="R3" t="n">
-        <v>242</v>
-      </c>
-      <c r="S3" t="n">
-        <v>220</v>
-      </c>
-      <c r="T3" t="n">
-        <v>4140142</v>
-      </c>
-      <c r="U3" t="n">
-        <v>62</v>
-      </c>
-      <c r="V3" t="n">
-        <v>3</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -707,77 +657,27 @@
           <t>ABBV</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/abbvie-inc-technical</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:38.971697</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>354</v>
-      </c>
-      <c r="G4" t="n">
-        <v>345</v>
-      </c>
-      <c r="H4" t="n">
-        <v>325</v>
-      </c>
-      <c r="I4" t="n">
-        <v>379</v>
-      </c>
-      <c r="J4" t="n">
-        <v>399</v>
-      </c>
-      <c r="K4" t="n">
-        <v>359</v>
-      </c>
-      <c r="L4" t="n">
-        <v>362</v>
-      </c>
-      <c r="M4" t="n">
-        <v>32</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-8</v>
-      </c>
-      <c r="O4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="P4" t="n">
-        <v>-2</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>384</v>
-      </c>
-      <c r="R4" t="n">
-        <v>362</v>
-      </c>
-      <c r="S4" t="n">
-        <v>340</v>
-      </c>
-      <c r="T4" t="n">
-        <v>2709762</v>
-      </c>
-      <c r="U4" t="n">
-        <v>32</v>
-      </c>
-      <c r="V4" t="n">
-        <v>3</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -785,77 +685,27 @@
           <t>ADBE</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/adobe-inc-technical</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:40.686815</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>176</v>
-      </c>
-      <c r="G5" t="n">
-        <v>165</v>
-      </c>
-      <c r="H5" t="n">
-        <v>155</v>
-      </c>
-      <c r="I5" t="n">
-        <v>201</v>
-      </c>
-      <c r="J5" t="n">
-        <v>211</v>
-      </c>
-      <c r="K5" t="n">
-        <v>181</v>
-      </c>
-      <c r="L5" t="n">
-        <v>180</v>
-      </c>
-      <c r="M5" t="n">
-        <v>53</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-7</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-4.5</v>
-      </c>
-      <c r="P5" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>206</v>
-      </c>
-      <c r="R5" t="n">
-        <v>183</v>
-      </c>
-      <c r="S5" t="n">
-        <v>160</v>
-      </c>
-      <c r="T5" t="n">
-        <v>8699583</v>
-      </c>
-      <c r="U5" t="n">
-        <v>53</v>
-      </c>
-      <c r="V5" t="n">
-        <v>4</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -863,77 +713,27 @@
           <t>ADI</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/analog-devices-technical</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:42.673470</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>274</v>
-      </c>
-      <c r="G6" t="n">
-        <v>255</v>
-      </c>
-      <c r="H6" t="n">
-        <v>240</v>
-      </c>
-      <c r="I6" t="n">
-        <v>289</v>
-      </c>
-      <c r="J6" t="n">
-        <v>304</v>
-      </c>
-      <c r="K6" t="n">
-        <v>269</v>
-      </c>
-      <c r="L6" t="n">
-        <v>270</v>
-      </c>
-      <c r="M6" t="n">
-        <v>62</v>
-      </c>
-      <c r="N6" t="n">
-        <v>2</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-0.5</v>
-      </c>
-      <c r="P6" t="n">
-        <v>-4</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>294</v>
-      </c>
-      <c r="R6" t="n">
-        <v>272</v>
-      </c>
-      <c r="S6" t="n">
-        <v>250</v>
-      </c>
-      <c r="T6" t="n">
-        <v>10933672</v>
-      </c>
-      <c r="U6" t="n">
-        <v>42</v>
-      </c>
-      <c r="V6" t="n">
-        <v>3</v>
-      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -941,77 +741,27 @@
           <t>ADSK</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/autodesk-inc-technical</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:43.838381</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>112</v>
-      </c>
-      <c r="G7" t="n">
-        <v>95</v>
-      </c>
-      <c r="H7" t="n">
-        <v>80</v>
-      </c>
-      <c r="I7" t="n">
-        <v>127</v>
-      </c>
-      <c r="J7" t="n">
-        <v>142</v>
-      </c>
-      <c r="K7" t="n">
-        <v>107</v>
-      </c>
-      <c r="L7" t="n">
-        <v>108</v>
-      </c>
-      <c r="M7" t="n">
-        <v>41</v>
-      </c>
-      <c r="N7" t="n">
-        <v>1</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-1.5</v>
-      </c>
-      <c r="P7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>132</v>
-      </c>
-      <c r="R7" t="n">
-        <v>111</v>
-      </c>
-      <c r="S7" t="n">
-        <v>90</v>
-      </c>
-      <c r="T7" t="n">
-        <v>6281011</v>
-      </c>
-      <c r="U7" t="n">
-        <v>31</v>
-      </c>
-      <c r="V7" t="n">
-        <v>2</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1019,77 +769,27 @@
           <t>ADYEY</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/adyen-nv-otc-technical</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:45.441807</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>226</v>
-      </c>
-      <c r="G8" t="n">
-        <v>195</v>
-      </c>
-      <c r="H8" t="n">
-        <v>190</v>
-      </c>
-      <c r="I8" t="n">
-        <v>241</v>
-      </c>
-      <c r="J8" t="n">
-        <v>246</v>
-      </c>
-      <c r="K8" t="n">
-        <v>221</v>
-      </c>
-      <c r="L8" t="n">
-        <v>218</v>
-      </c>
-      <c r="M8" t="n">
-        <v>48</v>
-      </c>
-      <c r="N8" t="n">
-        <v>8</v>
-      </c>
-      <c r="O8" t="n">
-        <v>-4.5</v>
-      </c>
-      <c r="P8" t="n">
-        <v>-2</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>246</v>
-      </c>
-      <c r="R8" t="n">
-        <v>218</v>
-      </c>
-      <c r="S8" t="n">
-        <v>190</v>
-      </c>
-      <c r="T8" t="n">
-        <v>5834618</v>
-      </c>
-      <c r="U8" t="n">
-        <v>38</v>
-      </c>
-      <c r="V8" t="n">
-        <v>9</v>
-      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1097,77 +797,27 @@
           <t>AEM</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/agnico-eagle-mines-technical</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:47.092396</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>402</v>
-      </c>
-      <c r="G9" t="n">
-        <v>385</v>
-      </c>
-      <c r="H9" t="n">
-        <v>375</v>
-      </c>
-      <c r="I9" t="n">
-        <v>427</v>
-      </c>
-      <c r="J9" t="n">
-        <v>437</v>
-      </c>
-      <c r="K9" t="n">
-        <v>407</v>
-      </c>
-      <c r="L9" t="n">
-        <v>406</v>
-      </c>
-      <c r="M9" t="n">
-        <v>36</v>
-      </c>
-      <c r="N9" t="n">
-        <v>-4</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-1.5</v>
-      </c>
-      <c r="P9" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>432</v>
-      </c>
-      <c r="R9" t="n">
-        <v>406</v>
-      </c>
-      <c r="S9" t="n">
-        <v>380</v>
-      </c>
-      <c r="T9" t="n">
-        <v>8205806</v>
-      </c>
-      <c r="U9" t="n">
-        <v>26</v>
-      </c>
-      <c r="V9" t="n">
-        <v>7</v>
-      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1175,77 +825,27 @@
           <t>AJG</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/arthur-j.-gallagher---co-technical</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:48.502007</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>450</v>
-      </c>
-      <c r="G10" t="n">
-        <v>435</v>
-      </c>
-      <c r="H10" t="n">
-        <v>420</v>
-      </c>
-      <c r="I10" t="n">
-        <v>465</v>
-      </c>
-      <c r="J10" t="n">
-        <v>480</v>
-      </c>
-      <c r="K10" t="n">
-        <v>445</v>
-      </c>
-      <c r="L10" t="n">
-        <v>446</v>
-      </c>
-      <c r="M10" t="n">
-        <v>60</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>-2.5</v>
-      </c>
-      <c r="P10" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>470</v>
-      </c>
-      <c r="R10" t="n">
-        <v>450</v>
-      </c>
-      <c r="S10" t="n">
-        <v>430</v>
-      </c>
-      <c r="T10" t="n">
-        <v>4003350</v>
-      </c>
-      <c r="U10" t="n">
-        <v>20</v>
-      </c>
-      <c r="V10" t="n">
-        <v>1</v>
-      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1253,77 +853,27 @@
           <t>ALL</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://www.investing.com/equities/allstate-corp-technical</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2025-09-24T15:10:50.048240</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>mock</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Mock data used due to network unavailability</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>312</v>
-      </c>
-      <c r="G11" t="n">
-        <v>305</v>
-      </c>
-      <c r="H11" t="n">
-        <v>290</v>
-      </c>
-      <c r="I11" t="n">
-        <v>337</v>
-      </c>
-      <c r="J11" t="n">
-        <v>352</v>
-      </c>
-      <c r="K11" t="n">
-        <v>317</v>
-      </c>
-      <c r="L11" t="n">
-        <v>324</v>
-      </c>
-      <c r="M11" t="n">
-        <v>51</v>
-      </c>
-      <c r="N11" t="n">
-        <v>-9</v>
-      </c>
-      <c r="O11" t="n">
-        <v>-1.5</v>
-      </c>
-      <c r="P11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>342</v>
-      </c>
-      <c r="R11" t="n">
-        <v>321</v>
-      </c>
-      <c r="S11" t="n">
-        <v>300</v>
-      </c>
-      <c r="T11" t="n">
-        <v>6499221</v>
-      </c>
-      <c r="U11" t="n">
-        <v>41</v>
-      </c>
-      <c r="V11" t="n">
-        <v>2</v>
-      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">

</xml_diff>

<commit_message>
Complete production debugging solution with enhanced error reporting and deployment guide
Co-authored-by: robertopotenza <138742974+robertopotenza@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-24T19:34:13.184636</t>
+          <t>2025-09-24T19:41:10.911695</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mock data used due to network unavailability</t>
+          <t>Mock data - PRODUCTION ISSUE: Network/DNS failure. Run production_debug.py for fixes.</t>
         </is>
       </c>
       <c r="F2" t="n">

</xml_diff>

<commit_message>
Implement fast network connectivity checks to prevent Chrome WebDriver hanging
Co-authored-by: robertopotenza <138742974+robertopotenza@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -558,7 +558,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-24T19:41:10.911695</t>
+          <t>2025-09-25T02:13:04.753829</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -568,7 +568,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mock data - PRODUCTION ISSUE: Network/DNS failure. Run production_debug.py for fixes.</t>
+          <t>Mock data - Network connectivity issue. Check internet connection.</t>
         </is>
       </c>
       <c r="F2" t="n">

</xml_diff>

<commit_message>
Final testing and verification complete
Co-authored-by: robertopotenza <138742974+robertopotenza@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -553,12 +553,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://www.investing.com/equities/aia-group-ltd-technical</t>
+          <t>Twelve Data API - AAGIY</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-09-25T02:13:04.753829</t>
+          <t>2025-09-25T14:54:20.824688</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -568,59 +568,59 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Mock data - Network connectivity issue. Check internet connection.</t>
+          <t>Mock data - No API key provided</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>386</v>
+        <v>447.2</v>
       </c>
       <c r="G2" t="n">
-        <v>355</v>
+        <v>434.07</v>
       </c>
       <c r="H2" t="n">
-        <v>350</v>
+        <v>419.27</v>
       </c>
       <c r="I2" t="n">
-        <v>401</v>
+        <v>462.01</v>
       </c>
       <c r="J2" t="n">
-        <v>406</v>
+        <v>475.14</v>
       </c>
       <c r="K2" t="n">
-        <v>381</v>
+        <v>449.59</v>
       </c>
       <c r="L2" t="n">
-        <v>378</v>
+        <v>464.8</v>
       </c>
       <c r="M2" t="n">
-        <v>68</v>
+        <v>26.62</v>
       </c>
       <c r="N2" t="n">
-        <v>8</v>
+        <v>1.8199</v>
       </c>
       <c r="O2" t="n">
-        <v>-4.5</v>
+        <v>1.0387</v>
       </c>
       <c r="P2" t="n">
-        <v>2</v>
+        <v>-0.2413</v>
       </c>
       <c r="Q2" t="n">
-        <v>406</v>
+        <v>478.27</v>
       </c>
       <c r="R2" t="n">
-        <v>378</v>
+        <v>448.04</v>
       </c>
       <c r="S2" t="n">
-        <v>350</v>
+        <v>396.29</v>
       </c>
       <c r="T2" t="n">
-        <v>9848278</v>
+        <v>2693979</v>
       </c>
       <c r="U2" t="n">
-        <v>48</v>
+        <v>59.67</v>
       </c>
       <c r="V2" t="n">
-        <v>9</v>
+        <v>3.2183</v>
       </c>
     </row>
     <row r="3">

</xml_diff>